<commit_message>
Atualização dados gerais 08/08
</commit_message>
<xml_diff>
--- a/Sergipe/data_general/ocupacao_uti.xlsx
+++ b/Sergipe/data_general/ocupacao_uti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adolfoguimaraes/Dev/DataViz/covid19-br/Vacinacao/Sergipe/data_general/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DE92EF-17F0-DF43-AA0D-627435BB0234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065C514C-AA86-1A48-8F5A-65B83D74188E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{397D0FB9-FECF-5A41-9117-EBA7D157FDD4}"/>
   </bookViews>
@@ -420,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C757372-1837-874B-976B-36795771F301}">
-  <dimension ref="A1:G220"/>
+  <dimension ref="A1:G222"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="C216" sqref="C216"/>
+      <selection activeCell="F213" sqref="F213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5353,7 +5353,7 @@
         <v>0.47368421052631576</v>
       </c>
       <c r="G197" s="2">
-        <f t="shared" ref="G197:G220" si="7">E197/D197</f>
+        <f t="shared" ref="G197:G222" si="7">E197/D197</f>
         <v>0.4485294117647059</v>
       </c>
     </row>
@@ -5749,7 +5749,7 @@
         <v>25</v>
       </c>
       <c r="F213" s="2">
-        <f t="shared" ref="F213:F220" si="8">C213/B213</f>
+        <f t="shared" ref="F213:F222" si="8">C213/B213</f>
         <v>0.35028248587570621</v>
       </c>
       <c r="G213" s="2">
@@ -5930,6 +5930,56 @@
       <c r="G220" s="2">
         <f t="shared" si="7"/>
         <v>0.26470588235294118</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A221" s="1">
+        <v>44415</v>
+      </c>
+      <c r="B221">
+        <v>137</v>
+      </c>
+      <c r="C221">
+        <v>47</v>
+      </c>
+      <c r="D221">
+        <v>68</v>
+      </c>
+      <c r="E221">
+        <v>18</v>
+      </c>
+      <c r="F221" s="2">
+        <f t="shared" si="8"/>
+        <v>0.34306569343065696</v>
+      </c>
+      <c r="G221" s="2">
+        <f t="shared" si="7"/>
+        <v>0.26470588235294118</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>44416</v>
+      </c>
+      <c r="B222">
+        <v>137</v>
+      </c>
+      <c r="C222">
+        <v>46</v>
+      </c>
+      <c r="D222">
+        <v>68</v>
+      </c>
+      <c r="E222">
+        <v>17</v>
+      </c>
+      <c r="F222" s="2">
+        <f t="shared" si="8"/>
+        <v>0.33576642335766421</v>
+      </c>
+      <c r="G222" s="2">
+        <f t="shared" si="7"/>
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>